<commit_message>
Conclusion in Manage notes-detail and Colisage
</commit_message>
<xml_diff>
--- a/COLISAGE_NAVITRANS_FINAL.xlsx
+++ b/COLISAGE_NAVITRANS_FINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoicTonba\source\PROJETS-WEB\sfx_predouanevtonba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA90ADB1-B11D-4E4D-BCD5-5C85313ECE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C922CC-F481-40FB-8F0E-F6B350C55862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,9 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="268">
   <si>
-    <t>Row_Key</t>
-  </si>
-  <si>
     <t>Command_No</t>
   </si>
   <si>
@@ -843,6 +840,9 @@
   </si>
   <si>
     <t>&gt;&gt; OFFER STEEL WELDING FLANGE FLAT FACE JIS MAT</t>
+  </si>
+  <si>
+    <t>Upload_Key</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1131,69 +1131,69 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>230217940</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1202,10 +1202,10 @@
         <v>8481808190</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2">
         <v>10</v>
@@ -1214,27 +1214,27 @@
         <v>563</v>
       </c>
       <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
         <v>22</v>
-      </c>
-      <c r="L2">
-        <v>100</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>230217940</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1243,10 +1243,10 @@
         <v>8481808190</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -1255,24 +1255,24 @@
         <v>1328</v>
       </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3" t="s">
         <v>22</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>230218659</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>26972</v>
@@ -1284,10 +1284,10 @@
         <v>8205200000</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -1296,24 +1296,24 @@
         <v>64.599999999999994</v>
       </c>
       <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
         <v>22</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>230218659</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>26972</v>
@@ -1325,10 +1325,10 @@
         <v>8205200000</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -1337,24 +1337,24 @@
         <v>64.599999999999994</v>
       </c>
       <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="M5" t="s">
         <v>22</v>
-      </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-      <c r="M5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>230218659</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>26972</v>
@@ -1366,10 +1366,10 @@
         <v>4009310090</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1378,24 +1378,24 @@
         <v>214.63</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L6">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>230218659</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>26972</v>
@@ -1407,10 +1407,10 @@
         <v>7312900000</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>30</v>
@@ -1419,24 +1419,24 @@
         <v>6.69</v>
       </c>
       <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7" t="s">
         <v>22</v>
-      </c>
-      <c r="L7">
-        <v>100</v>
-      </c>
-      <c r="M7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>230218659</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>26972</v>
@@ -1448,10 +1448,10 @@
         <v>4002999000</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8">
         <v>8</v>
@@ -1460,33 +1460,33 @@
         <v>157.88</v>
       </c>
       <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8" t="s">
         <v>22</v>
-      </c>
-      <c r="L8">
-        <v>100</v>
-      </c>
-      <c r="M8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>230218659</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>26972</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1498,18 +1498,18 @@
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>230220205</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>26975</v>
@@ -1521,10 +1521,10 @@
         <v>8204110000</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1533,24 +1533,24 @@
         <v>10.82</v>
       </c>
       <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10" t="s">
         <v>22</v>
-      </c>
-      <c r="L10">
-        <v>100</v>
-      </c>
-      <c r="M10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>230220205</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>26975</v>
@@ -1562,10 +1562,10 @@
         <v>8204120000</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1574,24 +1574,24 @@
         <v>30.4</v>
       </c>
       <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11" t="s">
         <v>22</v>
-      </c>
-      <c r="L11">
-        <v>100</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>230220205</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>26975</v>
@@ -1603,10 +1603,10 @@
         <v>4202929190</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12">
         <v>3</v>
@@ -1615,24 +1615,24 @@
         <v>93.54</v>
       </c>
       <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12" t="s">
         <v>22</v>
-      </c>
-      <c r="L12">
-        <v>100</v>
-      </c>
-      <c r="M12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>230220205</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13">
         <v>26975</v>
@@ -1644,10 +1644,10 @@
         <v>8204110000</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1656,24 +1656,24 @@
         <v>16.420000000000002</v>
       </c>
       <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13" t="s">
         <v>22</v>
-      </c>
-      <c r="L13">
-        <v>100</v>
-      </c>
-      <c r="M13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>230220335</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>251202439</v>
@@ -1685,10 +1685,10 @@
         <v>8204110000</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -1697,24 +1697,24 @@
         <v>71.36</v>
       </c>
       <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14" t="s">
         <v>22</v>
-      </c>
-      <c r="L14">
-        <v>100</v>
-      </c>
-      <c r="M14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>230220335</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>251202439</v>
@@ -1726,10 +1726,10 @@
         <v>8204110000</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -1738,24 +1738,24 @@
         <v>112</v>
       </c>
       <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15" t="s">
         <v>22</v>
-      </c>
-      <c r="L15">
-        <v>100</v>
-      </c>
-      <c r="M15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>230220335</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>251202439</v>
@@ -1764,10 +1764,10 @@
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1776,24 +1776,24 @@
         <v>185</v>
       </c>
       <c r="K16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17">
         <v>230220335</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>251202439</v>
@@ -1805,10 +1805,10 @@
         <v>90269000</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -1817,24 +1817,24 @@
         <v>72.42</v>
       </c>
       <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17">
+        <v>100</v>
+      </c>
+      <c r="M17" t="s">
         <v>22</v>
-      </c>
-      <c r="L17">
-        <v>100</v>
-      </c>
-      <c r="M17" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>230221345</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>251202501</v>
@@ -1846,10 +1846,10 @@
         <v>8506509090</v>
       </c>
       <c r="G18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18">
         <v>5</v>
@@ -1858,33 +1858,33 @@
         <v>93.65</v>
       </c>
       <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="M18" t="s">
         <v>22</v>
-      </c>
-      <c r="L18">
-        <v>100</v>
-      </c>
-      <c r="M18" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19">
         <v>230221345</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>251202501</v>
       </c>
       <c r="G19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1893,39 +1893,39 @@
         <v>272.23</v>
       </c>
       <c r="K19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>23217811</v>
       </c>
       <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>58</v>
       </c>
       <c r="F20">
         <v>32141010</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20">
         <v>5</v>
@@ -1934,39 +1934,39 @@
         <v>184.07</v>
       </c>
       <c r="K20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L20">
         <v>100</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21">
         <v>23217811</v>
       </c>
       <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F21">
         <v>73182100</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1975,39 +1975,39 @@
         <v>65.02</v>
       </c>
       <c r="K21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21">
         <v>100</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B22">
         <v>23217811</v>
       </c>
       <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" t="s">
-        <v>57</v>
-      </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22">
         <v>76169990</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -2016,36 +2016,36 @@
         <v>145.32</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L22">
         <v>100</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B23">
         <v>23217811</v>
       </c>
       <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="D23" t="s">
-        <v>57</v>
-      </c>
       <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
         <v>70</v>
       </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
       <c r="H23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -2057,33 +2057,33 @@
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1">
         <v>230220542</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1">
         <v>25030800027104</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="1">
         <v>85361090</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24" s="1">
         <v>3</v>
@@ -2092,13 +2092,13 @@
         <v>149.34</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L24" s="1">
         <v>100</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="1"/>
@@ -2107,28 +2107,28 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1">
         <v>230220542</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="1">
         <v>25030800027104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="1">
         <v>85393190</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I25" s="1">
         <v>100</v>
@@ -2137,13 +2137,13 @@
         <v>0.77</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L25" s="1">
         <v>100</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="1"/>
@@ -2152,13 +2152,13 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1">
         <v>230220542</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1">
         <v>25030800027104</v>
@@ -2168,10 +2168,10 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -2184,7 +2184,7 @@
         <v>100</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -2193,13 +2193,13 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1">
         <v>230215837</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D27" s="1">
         <v>2500634</v>
@@ -2211,10 +2211,10 @@
         <v>84139100</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I27" s="1">
         <v>4</v>
@@ -2223,13 +2223,13 @@
         <v>1377</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L27" s="1">
         <v>100</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="1">
@@ -2242,13 +2242,13 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="1">
         <v>230215837</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D28" s="1">
         <v>2500634</v>
@@ -2256,10 +2256,10 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I28" s="1">
         <v>1</v>
@@ -2268,13 +2268,13 @@
         <v>350</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L28" s="1">
         <v>0</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="1"/>
@@ -2283,28 +2283,28 @@
     </row>
     <row r="29" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="F29" s="4">
         <v>6305321900</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I29" s="4">
         <v>100</v>
@@ -2313,13 +2313,13 @@
         <v>21.15</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L29" s="1">
         <v>100</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N29" s="6"/>
       <c r="O29" s="4">
@@ -2334,16 +2334,16 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="1">
         <v>230209561</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -2352,10 +2352,10 @@
         <v>73079319</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I30" s="1">
         <v>10</v>
@@ -2364,13 +2364,13 @@
         <v>13.6</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L30" s="1">
         <v>100</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="1"/>
@@ -2379,16 +2379,16 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31" s="1">
         <v>230209561</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -2397,10 +2397,10 @@
         <v>73079319</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I31" s="1">
         <v>10</v>
@@ -2409,13 +2409,13 @@
         <v>31.6</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L31" s="1">
         <v>100</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="1"/>
@@ -2424,16 +2424,16 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B32" s="1">
         <v>230209561</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E32" s="1">
         <v>3</v>
@@ -2442,10 +2442,10 @@
         <v>73079100</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I32" s="1">
         <v>19</v>
@@ -2454,13 +2454,13 @@
         <v>27.74</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L32" s="1">
         <v>100</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="1"/>
@@ -2469,16 +2469,16 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="1">
         <v>230209561</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E33" s="1">
         <v>4</v>
@@ -2487,10 +2487,10 @@
         <v>73079319</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I33" s="1">
         <v>18</v>
@@ -2499,13 +2499,13 @@
         <v>43.99</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L33" s="1">
         <v>100</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="1"/>
@@ -2514,14 +2514,14 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
@@ -2529,7 +2529,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I34" s="1">
         <v>1</v>
@@ -2542,7 +2542,7 @@
         <v>100</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="1"/>
@@ -2551,28 +2551,28 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F35" s="1">
         <v>6305321900</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I35" s="1">
         <v>100</v>
@@ -2581,13 +2581,13 @@
         <v>21.15</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L35" s="1">
         <v>100</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="1">
@@ -2602,28 +2602,28 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F36" s="1">
         <v>6305321900</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I36" s="1">
         <v>60</v>
@@ -2632,13 +2632,13 @@
         <v>21.15</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L36" s="1">
         <v>100</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N36" s="3"/>
       <c r="O36" s="1">
@@ -2653,28 +2653,28 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B37" s="1">
         <v>230219361</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="F37" s="1">
         <v>84833080</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I37" s="1">
         <v>2</v>
@@ -2683,13 +2683,13 @@
         <v>57.49</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L37" s="1">
         <v>100</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N37" s="3"/>
       <c r="O37" s="1"/>
@@ -2698,26 +2698,26 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B38" s="1">
         <v>230219361</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I38" s="1">
         <v>1</v>
@@ -2730,7 +2730,7 @@
         <v>100</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N38" s="3"/>
       <c r="O38" s="1"/>
@@ -2739,13 +2739,13 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39">
         <v>230216486</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39">
         <v>26929</v>
@@ -2757,36 +2757,36 @@
         <v>8301409000</v>
       </c>
       <c r="G39" t="s">
+        <v>117</v>
+      </c>
+      <c r="H39" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39">
+        <v>20</v>
+      </c>
+      <c r="J39" t="s">
         <v>118</v>
       </c>
-      <c r="H39" t="s">
-        <v>21</v>
-      </c>
-      <c r="I39">
-        <v>20</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>119</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39">
+        <v>100</v>
+      </c>
+      <c r="M39" t="s">
         <v>120</v>
-      </c>
-      <c r="L39">
-        <v>100</v>
-      </c>
-      <c r="M39" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B40">
         <v>230216486</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40">
         <v>26929</v>
@@ -2798,68 +2798,68 @@
         <v>8301409000</v>
       </c>
       <c r="G40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I40">
         <v>20</v>
       </c>
       <c r="J40" t="s">
+        <v>118</v>
+      </c>
+      <c r="K40" t="s">
         <v>119</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40">
+        <v>100</v>
+      </c>
+      <c r="M40" t="s">
         <v>120</v>
-      </c>
-      <c r="L40">
-        <v>100</v>
-      </c>
-      <c r="M40" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41">
         <v>230216486</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D41">
         <v>26929</v>
       </c>
       <c r="G41" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41" t="s">
         <v>125</v>
-      </c>
-      <c r="H41" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41" t="s">
-        <v>126</v>
       </c>
       <c r="L41">
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B42">
         <v>230220187</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D42">
         <v>26930</v>
@@ -2871,36 +2871,36 @@
         <v>9603500000</v>
       </c>
       <c r="G42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42">
+        <v>20</v>
+      </c>
+      <c r="J42" t="s">
         <v>128</v>
       </c>
-      <c r="H42" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42">
-        <v>20</v>
-      </c>
-      <c r="J42" t="s">
-        <v>129</v>
-      </c>
       <c r="K42" t="s">
+        <v>119</v>
+      </c>
+      <c r="L42">
+        <v>100</v>
+      </c>
+      <c r="M42" t="s">
         <v>120</v>
-      </c>
-      <c r="L42">
-        <v>100</v>
-      </c>
-      <c r="M42" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43">
         <v>230220187</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D43">
         <v>26930</v>
@@ -2912,36 +2912,36 @@
         <v>9017809000</v>
       </c>
       <c r="G43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H43" t="s">
+        <v>20</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43" t="s">
         <v>131</v>
       </c>
-      <c r="H43" t="s">
+      <c r="K43" t="s">
         <v>21</v>
       </c>
-      <c r="I43">
-        <v>1</v>
-      </c>
-      <c r="J43" t="s">
-        <v>132</v>
-      </c>
-      <c r="K43" t="s">
-        <v>22</v>
-      </c>
       <c r="L43">
         <v>100</v>
       </c>
       <c r="M43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B44">
         <v>230220187</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D44">
         <v>26930</v>
@@ -2953,68 +2953,68 @@
         <v>8207309000</v>
       </c>
       <c r="G44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
         <v>134</v>
       </c>
-      <c r="H44" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="J44" t="s">
-        <v>135</v>
-      </c>
       <c r="K44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L44">
         <v>100</v>
       </c>
       <c r="M44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45">
         <v>230220187</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D45">
         <v>26930</v>
       </c>
       <c r="G45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I45">
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L45">
         <v>0</v>
       </c>
       <c r="M45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B46">
         <v>9928776</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46">
         <v>57747262</v>
@@ -3023,42 +3023,42 @@
         <v>38249098</v>
       </c>
       <c r="G46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I46">
         <v>15</v>
       </c>
       <c r="J46" t="s">
+        <v>140</v>
+      </c>
+      <c r="K46" t="s">
+        <v>21</v>
+      </c>
+      <c r="L46">
+        <v>100</v>
+      </c>
+      <c r="M46" t="s">
+        <v>120</v>
+      </c>
+      <c r="O46" t="s">
         <v>141</v>
       </c>
-      <c r="K46" t="s">
-        <v>22</v>
-      </c>
-      <c r="L46">
-        <v>100</v>
-      </c>
-      <c r="M46" t="s">
-        <v>121</v>
-      </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>142</v>
-      </c>
-      <c r="P46" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B47">
         <v>230220886</v>
       </c>
       <c r="C47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D47">
         <v>26961</v>
@@ -3070,36 +3070,36 @@
         <v>9608200000</v>
       </c>
       <c r="G47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I47">
         <v>4</v>
       </c>
       <c r="J47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L47">
         <v>100</v>
       </c>
       <c r="M47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B48">
         <v>230220886</v>
       </c>
       <c r="C48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D48">
         <v>26961</v>
@@ -3111,36 +3111,36 @@
         <v>9608200000</v>
       </c>
       <c r="G48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I48">
         <v>4</v>
       </c>
       <c r="J48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L48">
         <v>100</v>
       </c>
       <c r="M48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B49">
         <v>230220886</v>
       </c>
       <c r="C49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D49">
         <v>26961</v>
@@ -3152,36 +3152,36 @@
         <v>9608200000</v>
       </c>
       <c r="G49" t="s">
+        <v>150</v>
+      </c>
+      <c r="H49" t="s">
         <v>151</v>
-      </c>
-      <c r="H49" t="s">
-        <v>152</v>
       </c>
       <c r="I49">
         <v>4</v>
       </c>
       <c r="J49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L49">
         <v>100</v>
       </c>
       <c r="M49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B50">
         <v>230220886</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D50">
         <v>26961</v>
@@ -3193,36 +3193,36 @@
         <v>9608200000</v>
       </c>
       <c r="G50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I50">
         <v>4</v>
       </c>
       <c r="J50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L50">
         <v>100</v>
       </c>
       <c r="M50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B51">
         <v>230220886</v>
       </c>
       <c r="C51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D51">
         <v>26976</v>
@@ -3234,68 +3234,68 @@
         <v>4009420090</v>
       </c>
       <c r="G51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I51">
         <v>3</v>
       </c>
       <c r="J51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L51">
         <v>0</v>
       </c>
       <c r="M51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B52">
         <v>230220886</v>
       </c>
       <c r="C52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D52">
         <v>26976</v>
       </c>
       <c r="G52" t="s">
+        <v>158</v>
+      </c>
+      <c r="H52" t="s">
+        <v>20</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
         <v>159</v>
-      </c>
-      <c r="H52" t="s">
-        <v>21</v>
-      </c>
-      <c r="I52">
-        <v>1</v>
-      </c>
-      <c r="J52" t="s">
-        <v>160</v>
       </c>
       <c r="L52">
         <v>0</v>
       </c>
       <c r="M52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53">
         <v>230220054</v>
       </c>
       <c r="C53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D53">
         <v>2512022463</v>
@@ -3307,25 +3307,25 @@
         <v>85153990</v>
       </c>
       <c r="G53" t="s">
+        <v>161</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53" t="s">
         <v>162</v>
       </c>
-      <c r="H53" t="s">
-        <v>21</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
-      </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>163</v>
-      </c>
-      <c r="K53" t="s">
-        <v>164</v>
       </c>
       <c r="L53">
         <v>0</v>
       </c>
       <c r="M53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O53">
         <v>80</v>
@@ -3333,13 +3333,13 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B54">
         <v>230220054</v>
       </c>
       <c r="C54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D54">
         <v>2512022463</v>
@@ -3351,25 +3351,25 @@
         <v>85153990</v>
       </c>
       <c r="G54" t="s">
+        <v>165</v>
+      </c>
+      <c r="H54" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54" t="s">
         <v>166</v>
       </c>
-      <c r="H54" t="s">
-        <v>21</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-      <c r="J54" t="s">
-        <v>167</v>
-      </c>
       <c r="K54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L54">
         <v>0</v>
       </c>
       <c r="M54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O54">
         <v>80</v>
@@ -3377,13 +3377,13 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B55">
         <v>230220054</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D55">
         <v>2512022463</v>
@@ -3392,10 +3392,10 @@
         <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I55">
         <v>1</v>
@@ -3407,18 +3407,18 @@
         <v>0</v>
       </c>
       <c r="M55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B56">
         <v>230218740</v>
       </c>
       <c r="C56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D56">
         <v>26928</v>
@@ -3430,36 +3430,36 @@
         <v>82041200000</v>
       </c>
       <c r="G56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I56">
         <v>2</v>
       </c>
       <c r="J56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L56">
         <v>100</v>
       </c>
       <c r="M56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57">
         <v>230218740</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D57">
         <v>26928</v>
@@ -3471,36 +3471,36 @@
         <v>8201909100</v>
       </c>
       <c r="G57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I57">
         <v>4</v>
       </c>
       <c r="J57" t="s">
+        <v>172</v>
+      </c>
+      <c r="K57" t="s">
         <v>173</v>
       </c>
-      <c r="K57" t="s">
-        <v>174</v>
-      </c>
       <c r="L57">
         <v>100</v>
       </c>
       <c r="M57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B58">
         <v>230218740</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D58">
         <v>26928</v>
@@ -3512,36 +3512,36 @@
         <v>9026204000</v>
       </c>
       <c r="G58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I58">
         <v>5</v>
       </c>
       <c r="J58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L58">
         <v>0</v>
       </c>
       <c r="M58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B59">
         <v>230217557</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D59">
         <v>230217557</v>
@@ -3553,39 +3553,39 @@
         <v>8537109199</v>
       </c>
       <c r="G59" t="s">
+        <v>179</v>
+      </c>
+      <c r="H59" t="s">
+        <v>20</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
         <v>180</v>
       </c>
-      <c r="H59" t="s">
-        <v>21</v>
-      </c>
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
         <v>181</v>
-      </c>
-      <c r="K59" t="s">
-        <v>182</v>
       </c>
       <c r="L59">
         <v>0</v>
       </c>
       <c r="M59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B60">
         <v>230217557</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D60">
         <v>230217557</v>
@@ -3594,33 +3594,33 @@
         <v>3</v>
       </c>
       <c r="G60" t="s">
+        <v>184</v>
+      </c>
+      <c r="H60" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
         <v>185</v>
-      </c>
-      <c r="H60" t="s">
-        <v>21</v>
-      </c>
-      <c r="I60">
-        <v>1</v>
-      </c>
-      <c r="J60" t="s">
-        <v>186</v>
       </c>
       <c r="L60">
         <v>0</v>
       </c>
       <c r="M60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B61">
         <v>230219198</v>
       </c>
       <c r="C61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D61">
         <v>26973</v>
@@ -3632,36 +3632,36 @@
         <v>8213000000</v>
       </c>
       <c r="G61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I61">
         <v>4</v>
       </c>
       <c r="J61" t="s">
+        <v>188</v>
+      </c>
+      <c r="K61" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61">
+        <v>100</v>
+      </c>
+      <c r="M61" t="s">
         <v>189</v>
-      </c>
-      <c r="K61" t="s">
-        <v>22</v>
-      </c>
-      <c r="L61">
-        <v>100</v>
-      </c>
-      <c r="M61" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B62">
         <v>230219198</v>
       </c>
       <c r="C62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D62">
         <v>26973</v>
@@ -3673,45 +3673,45 @@
         <v>3402901090</v>
       </c>
       <c r="G62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I62">
         <v>8</v>
       </c>
       <c r="J62" t="s">
+        <v>192</v>
+      </c>
+      <c r="K62" t="s">
         <v>193</v>
       </c>
-      <c r="K62" t="s">
-        <v>194</v>
-      </c>
       <c r="L62">
         <v>100</v>
       </c>
       <c r="M62" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B63">
         <v>230219198</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D63">
         <v>26973</v>
       </c>
       <c r="G63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I63">
         <v>1</v>
@@ -3723,18 +3723,18 @@
         <v>0</v>
       </c>
       <c r="M63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B64">
         <v>230220548</v>
       </c>
       <c r="C64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D64">
         <v>26974</v>
@@ -3746,36 +3746,36 @@
         <v>7310299090</v>
       </c>
       <c r="G64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I64">
         <v>12</v>
       </c>
       <c r="J64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L64">
         <v>100</v>
       </c>
       <c r="M64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B65">
         <v>230220548</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D65">
         <v>26974</v>
@@ -3784,10 +3784,10 @@
         <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -3799,147 +3799,147 @@
         <v>0</v>
       </c>
       <c r="M65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B66">
         <v>230216718</v>
       </c>
       <c r="C66" t="s">
+        <v>204</v>
+      </c>
+      <c r="D66" t="s">
         <v>205</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>206</v>
-      </c>
-      <c r="E66" t="s">
-        <v>207</v>
       </c>
       <c r="F66">
         <v>84189990</v>
       </c>
       <c r="G66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I66">
         <v>4</v>
       </c>
       <c r="J66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L66">
         <v>100</v>
       </c>
       <c r="M66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B67">
         <v>230216718</v>
       </c>
       <c r="C67" t="s">
+        <v>204</v>
+      </c>
+      <c r="D67" t="s">
         <v>205</v>
       </c>
-      <c r="D67" t="s">
-        <v>206</v>
-      </c>
       <c r="E67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F67">
         <v>89079000</v>
       </c>
       <c r="G67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I67">
         <v>2</v>
       </c>
       <c r="J67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L67">
         <v>100</v>
       </c>
       <c r="M67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B68">
         <v>230216718</v>
       </c>
       <c r="C68" t="s">
+        <v>204</v>
+      </c>
+      <c r="D68" t="s">
         <v>205</v>
       </c>
-      <c r="D68" t="s">
-        <v>206</v>
-      </c>
       <c r="E68" t="s">
+        <v>214</v>
+      </c>
+      <c r="G68" t="s">
         <v>215</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
+        <v>20</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68" t="s">
         <v>216</v>
-      </c>
-      <c r="H68" t="s">
-        <v>21</v>
-      </c>
-      <c r="I68">
-        <v>1</v>
-      </c>
-      <c r="J68" t="s">
-        <v>217</v>
       </c>
       <c r="L68">
         <v>0</v>
       </c>
       <c r="M68" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B69">
         <v>230216718</v>
       </c>
       <c r="C69" t="s">
+        <v>204</v>
+      </c>
+      <c r="D69" t="s">
         <v>205</v>
       </c>
-      <c r="D69" t="s">
-        <v>206</v>
-      </c>
       <c r="E69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G69" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -3951,21 +3951,21 @@
         <v>0</v>
       </c>
       <c r="M69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B70">
         <v>230218873</v>
       </c>
       <c r="C70" t="s">
+        <v>220</v>
+      </c>
+      <c r="D70" t="s">
         <v>221</v>
-      </c>
-      <c r="D70" t="s">
-        <v>222</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -3974,39 +3974,39 @@
         <v>84139100</v>
       </c>
       <c r="G70" t="s">
+        <v>222</v>
+      </c>
+      <c r="H70" t="s">
+        <v>20</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70" t="s">
         <v>223</v>
       </c>
-      <c r="H70" t="s">
-        <v>21</v>
-      </c>
-      <c r="I70">
-        <v>1</v>
-      </c>
-      <c r="J70" t="s">
-        <v>224</v>
-      </c>
       <c r="K70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L70">
         <v>100</v>
       </c>
       <c r="M70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B71">
         <v>230218873</v>
       </c>
       <c r="C71" t="s">
+        <v>220</v>
+      </c>
+      <c r="D71" t="s">
         <v>221</v>
-      </c>
-      <c r="D71" t="s">
-        <v>222</v>
       </c>
       <c r="E71">
         <v>2</v>
@@ -4015,39 +4015,39 @@
         <v>84139100</v>
       </c>
       <c r="G71" t="s">
+        <v>225</v>
+      </c>
+      <c r="H71" t="s">
+        <v>20</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71" t="s">
         <v>226</v>
       </c>
-      <c r="H71" t="s">
-        <v>21</v>
-      </c>
-      <c r="I71">
-        <v>1</v>
-      </c>
-      <c r="J71" t="s">
-        <v>227</v>
-      </c>
       <c r="K71" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L71">
         <v>100</v>
       </c>
       <c r="M71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B72">
         <v>230218873</v>
       </c>
       <c r="C72" t="s">
+        <v>220</v>
+      </c>
+      <c r="D72" t="s">
         <v>221</v>
-      </c>
-      <c r="D72" t="s">
-        <v>222</v>
       </c>
       <c r="E72">
         <v>3</v>
@@ -4056,48 +4056,48 @@
         <v>84139100</v>
       </c>
       <c r="G72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I72">
         <v>3</v>
       </c>
       <c r="J72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L72">
         <v>100</v>
       </c>
       <c r="M72" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B73">
         <v>230218873</v>
       </c>
       <c r="C73" t="s">
+        <v>220</v>
+      </c>
+      <c r="D73" t="s">
         <v>221</v>
-      </c>
-      <c r="D73" t="s">
-        <v>222</v>
       </c>
       <c r="E73">
         <v>5</v>
       </c>
       <c r="G73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I73">
         <v>1</v>
@@ -4106,27 +4106,27 @@
         <v>310</v>
       </c>
       <c r="K73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L73">
         <v>0</v>
       </c>
       <c r="M73" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B74">
         <v>230218873</v>
       </c>
       <c r="C74" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" t="s">
         <v>221</v>
-      </c>
-      <c r="D74" t="s">
-        <v>222</v>
       </c>
       <c r="E74">
         <v>4</v>
@@ -4135,39 +4135,39 @@
         <v>84139100</v>
       </c>
       <c r="G74" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I74">
         <v>3</v>
       </c>
       <c r="J74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L74">
         <v>100</v>
       </c>
       <c r="M74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B75" t="s">
+        <v>234</v>
+      </c>
+      <c r="C75" t="s">
         <v>235</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>236</v>
-      </c>
-      <c r="D75" t="s">
-        <v>237</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -4176,39 +4176,39 @@
         <v>591190900</v>
       </c>
       <c r="G75" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I75">
         <v>10</v>
       </c>
       <c r="J75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L75">
         <v>100</v>
       </c>
       <c r="M75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>233</v>
+      </c>
+      <c r="B76" t="s">
         <v>234</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>235</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>236</v>
-      </c>
-      <c r="D76" t="s">
-        <v>237</v>
       </c>
       <c r="E76">
         <v>2</v>
@@ -4217,39 +4217,39 @@
         <v>591190900</v>
       </c>
       <c r="G76" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I76">
         <v>10</v>
       </c>
       <c r="J76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L76">
         <v>100</v>
       </c>
       <c r="M76" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B77" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" t="s">
         <v>235</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>236</v>
-      </c>
-      <c r="D77" t="s">
-        <v>237</v>
       </c>
       <c r="E77">
         <v>3</v>
@@ -4258,39 +4258,39 @@
         <v>591190900</v>
       </c>
       <c r="G77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I77">
         <v>12</v>
       </c>
       <c r="J77" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L77">
         <v>100</v>
       </c>
       <c r="M77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B78" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" t="s">
         <v>235</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>236</v>
-      </c>
-      <c r="D78" t="s">
-        <v>237</v>
       </c>
       <c r="E78">
         <v>4</v>
@@ -4299,10 +4299,10 @@
         <v>591190900</v>
       </c>
       <c r="G78" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I78">
         <v>1</v>
@@ -4311,39 +4311,39 @@
         <v>250</v>
       </c>
       <c r="K78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L78">
         <v>0</v>
       </c>
       <c r="M78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B79">
         <v>9776207</v>
       </c>
       <c r="C79" t="s">
+        <v>246</v>
+      </c>
+      <c r="D79" t="s">
         <v>247</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>248</v>
-      </c>
-      <c r="E79" t="s">
-        <v>249</v>
       </c>
       <c r="F79">
         <v>87168000</v>
       </c>
       <c r="G79" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I79">
         <v>1</v>
@@ -4352,39 +4352,39 @@
         <v>792</v>
       </c>
       <c r="K79" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L79">
         <v>100</v>
       </c>
       <c r="M79" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B80">
         <v>9776207</v>
       </c>
       <c r="C80" t="s">
+        <v>246</v>
+      </c>
+      <c r="D80" t="s">
         <v>247</v>
       </c>
-      <c r="D80" t="s">
-        <v>248</v>
-      </c>
       <c r="E80" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F80">
         <v>87168000</v>
       </c>
       <c r="G80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I80">
         <v>1</v>
@@ -4393,27 +4393,27 @@
         <v>942.4</v>
       </c>
       <c r="K80" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L80">
         <v>100</v>
       </c>
       <c r="M80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B81">
         <v>230220374</v>
       </c>
       <c r="C81" t="s">
+        <v>261</v>
+      </c>
+      <c r="D81" t="s">
         <v>262</v>
-      </c>
-      <c r="D81" t="s">
-        <v>263</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -4422,10 +4422,10 @@
         <v>85049090</v>
       </c>
       <c r="G81" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I81">
         <v>1</v>
@@ -4434,27 +4434,27 @@
         <v>1403.23</v>
       </c>
       <c r="K81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L81">
         <v>100</v>
       </c>
       <c r="M81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B82">
         <v>230220374</v>
       </c>
       <c r="C82" t="s">
+        <v>261</v>
+      </c>
+      <c r="D82" t="s">
         <v>262</v>
-      </c>
-      <c r="D82" t="s">
-        <v>263</v>
       </c>
       <c r="E82">
         <v>2</v>
@@ -4463,10 +4463,10 @@
         <v>73079100</v>
       </c>
       <c r="G82" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I82">
         <v>2</v>
@@ -4475,33 +4475,33 @@
         <v>150.79</v>
       </c>
       <c r="K82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L82">
         <v>100</v>
       </c>
       <c r="M82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B83">
         <v>230220374</v>
       </c>
       <c r="C83" t="s">
+        <v>261</v>
+      </c>
+      <c r="D83" t="s">
         <v>262</v>
       </c>
-      <c r="D83" t="s">
-        <v>263</v>
-      </c>
       <c r="G83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I83">
         <v>1</v>
@@ -4510,13 +4510,13 @@
         <v>150</v>
       </c>
       <c r="K83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L83">
         <v>0</v>
       </c>
       <c r="M83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAJ-09-02-2026-BD-SFX_PreDouane.sql and optimization for missing values dialog (hscode, pays, devises, regimeDeclaration)
</commit_message>
<xml_diff>
--- a/COLISAGE_NAVITRANS_FINAL.xlsx
+++ b/COLISAGE_NAVITRANS_FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoicTonba\source\PROJETS-WEB\sfx_predouanevtonba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C922CC-F481-40FB-8F0E-F6B350C55862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043E0CC6-BFBB-41CC-85C0-183ECBE202DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="270">
   <si>
     <t>Command_No</t>
   </si>
@@ -843,6 +843,12 @@
   </si>
   <si>
     <t>Upload_Key</t>
+  </si>
+  <si>
+    <t>EF004</t>
+  </si>
+  <si>
+    <t>Bourgies d'afrique</t>
   </si>
 </sst>
 </file>
@@ -1106,20 +1112,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="L88" sqref="L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.75" customWidth="1"/>
-    <col min="3" max="3" width="25.75" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
     <col min="4" max="4" width="15.75" customWidth="1"/>
     <col min="5" max="5" width="11.875" customWidth="1"/>
     <col min="6" max="6" width="12.75" customWidth="1"/>
-    <col min="7" max="7" width="40.75" customWidth="1"/>
+    <col min="7" max="7" width="26.375" customWidth="1"/>
     <col min="8" max="8" width="10.75" customWidth="1"/>
     <col min="9" max="11" width="15.75" customWidth="1"/>
     <col min="12" max="12" width="20.75" customWidth="1"/>
@@ -1363,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>4009310090</v>
+        <v>40092310090</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -1404,7 +1410,7 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>7312900000</v>
+        <v>73129030000</v>
       </c>
       <c r="G7" t="s">
         <v>32</v>
@@ -1442,10 +1448,10 @@
         <v>26972</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>4002999000</v>
+        <v>40029199000</v>
       </c>
       <c r="G8" t="s">
         <v>34</v>
@@ -4516,6 +4522,47 @@
         <v>0</v>
       </c>
       <c r="M83" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>268</v>
+      </c>
+      <c r="B84">
+        <v>230220374</v>
+      </c>
+      <c r="C84" t="s">
+        <v>261</v>
+      </c>
+      <c r="D84" t="s">
+        <v>262</v>
+      </c>
+      <c r="E84">
+        <v>3</v>
+      </c>
+      <c r="F84">
+        <v>3173079100</v>
+      </c>
+      <c r="G84" t="s">
+        <v>269</v>
+      </c>
+      <c r="H84" t="s">
+        <v>20</v>
+      </c>
+      <c r="I84">
+        <v>2</v>
+      </c>
+      <c r="J84">
+        <v>134</v>
+      </c>
+      <c r="K84" t="s">
+        <v>201</v>
+      </c>
+      <c r="L84">
+        <v>100</v>
+      </c>
+      <c r="M84" t="s">
         <v>189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified tauxDC at tauxRegime update Manage Clients,RegimeClients,RegimeDeclaration and database in sql server
</commit_message>
<xml_diff>
--- a/COLISAGE_NAVITRANS_FINAL.xlsx
+++ b/COLISAGE_NAVITRANS_FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoicTonba\source\PROJETS-WEB\sfx_predouanevtonba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043E0CC6-BFBB-41CC-85C0-183ECBE202DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8B28BE-D06C-473A-96C5-3756A504EE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="L88" sqref="L88"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>